<commit_message>
create_nodes not in venv anymore
</commit_message>
<xml_diff>
--- a/distances.xlsx
+++ b/distances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kilian\TUM\TUM\Bachelor Thesis\Code\distances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kilian\TUM\TUM\Bachelor Thesis\Code\simulated annealing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A5C9AD-1BA7-4197-9309-582F8C3C8AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC98E027-44E4-4A56-819D-9766535CCD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3055,34 +3055,16 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I52" s="4">
-        <f>MAX(I2:I50)</f>
-        <v>37.302840000000003</v>
-      </c>
-      <c r="J52" s="4">
-        <f>MAX(J2:J50)</f>
-        <v>37.006979999999999</v>
-      </c>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I53" s="4">
-        <f>MIN(I2:I50)</f>
-        <v>37.054839999999999</v>
-      </c>
-      <c r="J53" s="4">
-        <f>MIN(J2:J50)</f>
-        <v>36.698639999999997</v>
-      </c>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I54" s="4">
-        <f>I52-I53</f>
-        <v>0.24800000000000466</v>
-      </c>
-      <c r="J54" s="4">
-        <f>J52-J53</f>
-        <v>0.30834000000000117</v>
-      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
first working version of vrp with revisits
</commit_message>
<xml_diff>
--- a/distances.xlsx
+++ b/distances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kilian\TUM\TUM\Bachelor Thesis\Code\simulated annealing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC98E027-44E4-4A56-819D-9766535CCD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F90A2-2141-4A18-977E-255431779AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -956,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
@@ -3076,13 +3076,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX50"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="38.88671875" style="5" customWidth="1"/>
     <col min="2" max="50" width="15.77734375" style="5" customWidth="1"/>
     <col min="51" max="51" width="6.44140625" customWidth="1"/>
   </cols>

</xml_diff>